<commit_message>
Works CL at BE
</commit_message>
<xml_diff>
--- a/Entity/BESensorLessParams_413532721.xlsx
+++ b/Entity/BESensorLessParams_413532721.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SensorLess\Software\Kvaser\BETest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAD21CE-FAB8-4182-844A-F46A4F669669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DE9391-12C7-413B-917E-AE491012F6D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DefaultPars" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="235">
   <si>
     <t>Name</t>
   </si>
@@ -361,6 +361,9 @@
     <t>ClaControlPars.KeHz</t>
   </si>
   <si>
+    <t>Anti windup scale for current control</t>
+  </si>
+  <si>
     <t>ControlPars.I2tCurTime</t>
   </si>
   <si>
@@ -638,6 +641,54 @@
   </si>
   <si>
     <t>Time for initial rotor stabilization</t>
+  </si>
+  <si>
+    <t>SLPars.Pars6Step.TransitionTime</t>
+  </si>
+  <si>
+    <t>Time for transition allowance on 6-step event</t>
+  </si>
+  <si>
+    <t>SLPars.Pars6Step.SummingTime</t>
+  </si>
+  <si>
+    <t>Time for summing voltage / current for R estimate</t>
+  </si>
+  <si>
+    <t>SLPars.Pars6Step.MinimumCur4RCalc</t>
+  </si>
+  <si>
+    <t>Minimum current step for a well defined R evaluation</t>
+  </si>
+  <si>
+    <t>SLPars.Pars6Step.OpenLoopCurDiDtMax</t>
+  </si>
+  <si>
+    <t>Maximum current rise rate for open loop mode</t>
+  </si>
+  <si>
+    <t>SLPars.Pars6Step.MaxStepTime</t>
+  </si>
+  <si>
+    <t>Maximum step time in 6 step mode</t>
+  </si>
+  <si>
+    <t>SLPars.Pars6Step.JOverKT</t>
+  </si>
+  <si>
+    <t>Plant dynamics normalizer</t>
+  </si>
+  <si>
+    <t>SLPars.Pars6Step.Har3Phase</t>
+  </si>
+  <si>
+    <t>Third harmonic angle correction phase</t>
+  </si>
+  <si>
+    <t>SLPars.Pars6Step.Har3Amp</t>
+  </si>
+  <si>
+    <t>Third harmonic angle correction amplitude</t>
   </si>
   <si>
     <t>ClaMailIn.StoTholdScale</t>
@@ -1000,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F85"/>
+      <selection sqref="A1:F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1285,10 +1336,10 @@
         <v>1000000</v>
       </c>
       <c r="E14">
-        <v>0.88</v>
+        <v>0.95</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1356,7 +1407,7 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C18">
         <v>9.9999999999999995E-8</v>
@@ -1368,7 +1419,7 @@
         <v>24</v>
       </c>
       <c r="F18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1376,7 +1427,7 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1388,7 +1439,7 @@
         <v>500</v>
       </c>
       <c r="F19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1396,7 +1447,7 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1408,7 +1459,7 @@
         <v>2000</v>
       </c>
       <c r="F20" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1505,7 +1556,7 @@
         <v>1</v>
       </c>
       <c r="E25">
-        <v>7.9229629629629997E-2</v>
+        <v>0.4118</v>
       </c>
       <c r="F25" t="s">
         <v>65</v>
@@ -1616,7 +1667,7 @@
         <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -1628,7 +1679,7 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1636,7 +1687,7 @@
         <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C32">
         <v>32</v>
@@ -1648,7 +1699,7 @@
         <v>1440</v>
       </c>
       <c r="F32" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1656,7 +1707,7 @@
         <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1668,7 +1719,7 @@
         <v>2.1</v>
       </c>
       <c r="F33" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1676,7 +1727,7 @@
         <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1688,7 +1739,7 @@
         <v>2.56</v>
       </c>
       <c r="F34" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1696,7 +1747,7 @@
         <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C35">
         <v>11</v>
@@ -1708,7 +1759,7 @@
         <v>19</v>
       </c>
       <c r="F35" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1716,7 +1767,7 @@
         <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C36">
         <v>11</v>
@@ -1728,7 +1779,7 @@
         <v>60</v>
       </c>
       <c r="F36" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1736,7 +1787,7 @@
         <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C37">
         <v>0.01</v>
@@ -1756,7 +1807,7 @@
         <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C38">
         <v>0.5</v>
@@ -1768,7 +1819,7 @@
         <v>22</v>
       </c>
       <c r="F38" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1776,7 +1827,7 @@
         <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C39">
         <v>1E-3</v>
@@ -1788,7 +1839,7 @@
         <v>3.3300000000000003E-2</v>
       </c>
       <c r="F39" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1836,7 +1887,7 @@
         <v>92</v>
       </c>
       <c r="B42" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C42">
         <v>15</v>
@@ -1848,7 +1899,7 @@
         <v>16.5</v>
       </c>
       <c r="F42" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1856,7 +1907,7 @@
         <v>93</v>
       </c>
       <c r="B43" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1868,7 +1919,7 @@
         <v>85</v>
       </c>
       <c r="F43" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1876,7 +1927,7 @@
         <v>94</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C44">
         <v>1E-3</v>
@@ -1888,7 +1939,7 @@
         <v>0.1</v>
       </c>
       <c r="F44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1896,7 +1947,7 @@
         <v>95</v>
       </c>
       <c r="B45" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C45">
         <v>1E-3</v>
@@ -1908,7 +1959,7 @@
         <v>3</v>
       </c>
       <c r="F45" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1916,7 +1967,7 @@
         <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C46">
         <v>1E-3</v>
@@ -1928,7 +1979,7 @@
         <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1936,7 +1987,7 @@
         <v>98</v>
       </c>
       <c r="B47" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C47">
         <v>1E-3</v>
@@ -1948,7 +1999,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="F47" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1956,7 +2007,7 @@
         <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C48">
         <v>1E-3</v>
@@ -1968,7 +2019,7 @@
         <v>0.1</v>
       </c>
       <c r="F48" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1976,7 +2027,7 @@
         <v>100</v>
       </c>
       <c r="B49" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C49">
         <v>1E-3</v>
@@ -1988,7 +2039,7 @@
         <v>0.1</v>
       </c>
       <c r="F49" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2008,7 +2059,7 @@
         <v>0.05</v>
       </c>
       <c r="F50" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2028,7 +2079,7 @@
         <v>0.1</v>
       </c>
       <c r="F51" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2036,19 +2087,19 @@
         <v>105</v>
       </c>
       <c r="B52" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C52">
         <v>0</v>
       </c>
       <c r="D52">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E52">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F52" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2056,7 +2107,7 @@
         <v>106</v>
       </c>
       <c r="B53" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2068,7 +2119,7 @@
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2076,7 +2127,7 @@
         <v>107</v>
       </c>
       <c r="B54" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -2088,7 +2139,7 @@
         <v>2</v>
       </c>
       <c r="F54" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2096,7 +2147,7 @@
         <v>110</v>
       </c>
       <c r="B55" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C55">
         <v>9.9999999999999995E-8</v>
@@ -2108,7 +2159,7 @@
         <v>0.13</v>
       </c>
       <c r="F55" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2116,7 +2167,7 @@
         <v>111</v>
       </c>
       <c r="B56" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C56">
         <v>9.9999999999999995E-8</v>
@@ -2128,7 +2179,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="F56" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2136,7 +2187,7 @@
         <v>112</v>
       </c>
       <c r="B57" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -2148,7 +2199,7 @@
         <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2156,7 +2207,7 @@
         <v>113</v>
       </c>
       <c r="B58" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -2168,7 +2219,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="F58" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2176,7 +2227,7 @@
         <v>114</v>
       </c>
       <c r="B59" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -2188,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="F59" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2196,7 +2247,7 @@
         <v>115</v>
       </c>
       <c r="B60" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C60">
         <v>9.9999999999999995E-8</v>
@@ -2208,7 +2259,7 @@
         <v>0.13</v>
       </c>
       <c r="F60" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2216,7 +2267,7 @@
         <v>116</v>
       </c>
       <c r="B61" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C61">
         <v>9.9999999999999995E-8</v>
@@ -2228,7 +2279,7 @@
         <v>7802.6</v>
       </c>
       <c r="F61" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2236,7 +2287,7 @@
         <v>117</v>
       </c>
       <c r="B62" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C62">
         <v>9.9999999999999995E-8</v>
@@ -2248,7 +2299,7 @@
         <v>149.0188</v>
       </c>
       <c r="F62" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2256,7 +2307,7 @@
         <v>118</v>
       </c>
       <c r="B63" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C63">
         <v>9.9999999999999995E-8</v>
@@ -2268,7 +2319,7 @@
         <v>50</v>
       </c>
       <c r="F63" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2276,7 +2327,7 @@
         <v>119</v>
       </c>
       <c r="B64" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C64">
         <v>9.9999999999999995E-8</v>
@@ -2288,7 +2339,7 @@
         <v>500</v>
       </c>
       <c r="F64" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2296,7 +2347,7 @@
         <v>120</v>
       </c>
       <c r="B65" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C65">
         <v>9.9999999999999995E-8</v>
@@ -2308,7 +2359,7 @@
         <v>0</v>
       </c>
       <c r="F65" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2316,7 +2367,7 @@
         <v>121</v>
       </c>
       <c r="B66" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C66">
         <v>9.9999999999999995E-8</v>
@@ -2328,7 +2379,7 @@
         <v>0.9</v>
       </c>
       <c r="F66" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2336,7 +2387,7 @@
         <v>122</v>
       </c>
       <c r="B67" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C67">
         <v>9.9999999999999995E-8</v>
@@ -2348,7 +2399,7 @@
         <v>3</v>
       </c>
       <c r="F67" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2356,7 +2407,7 @@
         <v>123</v>
       </c>
       <c r="B68" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C68">
         <v>9.9999999999999995E-8</v>
@@ -2368,7 +2419,7 @@
         <v>0.1</v>
       </c>
       <c r="F68" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2376,7 +2427,7 @@
         <v>124</v>
       </c>
       <c r="B69" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -2388,7 +2439,7 @@
         <v>0.17</v>
       </c>
       <c r="F69" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2396,7 +2447,7 @@
         <v>125</v>
       </c>
       <c r="B70" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C70">
         <v>-1</v>
@@ -2408,7 +2459,7 @@
         <v>-0.05</v>
       </c>
       <c r="F70" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2416,7 +2467,7 @@
         <v>126</v>
       </c>
       <c r="B71" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C71">
         <v>9.9999999999999995E-8</v>
@@ -2428,7 +2479,7 @@
         <v>4</v>
       </c>
       <c r="F71" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2436,7 +2487,7 @@
         <v>127</v>
       </c>
       <c r="B72" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C72">
         <v>9.9999999999999995E-8</v>
@@ -2448,7 +2499,7 @@
         <v>1</v>
       </c>
       <c r="F72" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2456,7 +2507,7 @@
         <v>128</v>
       </c>
       <c r="B73" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C73">
         <v>9.9999999999999995E-8</v>
@@ -2468,7 +2519,7 @@
         <v>3</v>
       </c>
       <c r="F73" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2476,7 +2527,7 @@
         <v>130</v>
       </c>
       <c r="B74" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C74">
         <v>9.9999999999999995E-8</v>
@@ -2488,7 +2539,7 @@
         <v>3</v>
       </c>
       <c r="F74" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2496,7 +2547,7 @@
         <v>131</v>
       </c>
       <c r="B75" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C75">
         <v>9.9999999999999995E-8</v>
@@ -2508,7 +2559,7 @@
         <v>3</v>
       </c>
       <c r="F75" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2516,7 +2567,7 @@
         <v>132</v>
       </c>
       <c r="B76" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C76">
         <v>9.9999999999999995E-8</v>
@@ -2528,7 +2579,7 @@
         <v>6</v>
       </c>
       <c r="F76" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2536,7 +2587,7 @@
         <v>133</v>
       </c>
       <c r="B77" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C77">
         <v>9.9999999999999995E-8</v>
@@ -2548,167 +2599,327 @@
         <v>1.5</v>
       </c>
       <c r="F77" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>239</v>
+        <v>134</v>
       </c>
       <c r="B78" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C78">
-        <v>-1.5</v>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="D78">
-        <v>1.5</v>
+        <v>0.01</v>
       </c>
       <c r="E78">
-        <v>1</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="F78" t="s">
-        <v>87</v>
+        <v>205</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>246</v>
+        <v>135</v>
       </c>
       <c r="B79" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C79">
-        <v>9.9999999999999995E-7</v>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="D79">
-        <v>99999999</v>
+        <v>0.01</v>
       </c>
       <c r="E79">
-        <v>200</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="F79" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>247</v>
+        <v>136</v>
       </c>
       <c r="B80" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C80">
-        <v>9.9999999999999995E-7</v>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="D80">
-        <v>0.99999998999999995</v>
+        <v>100</v>
       </c>
       <c r="E80">
-        <v>1.6659999999999999E-3</v>
+        <v>5</v>
       </c>
       <c r="F80" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>248</v>
+        <v>137</v>
       </c>
       <c r="B81" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="D81">
-        <v>0.99999998999999995</v>
+        <v>1000</v>
       </c>
       <c r="E81">
-        <v>1.25E-3</v>
+        <v>12</v>
       </c>
       <c r="F81" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>249</v>
+        <v>138</v>
       </c>
       <c r="B82" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="D82">
-        <v>9999.9999000000007</v>
+        <v>1000</v>
       </c>
       <c r="E82">
-        <v>0.45</v>
+        <v>0.1</v>
       </c>
       <c r="F82" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>250</v>
+        <v>139</v>
       </c>
       <c r="B83" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="D83">
-        <v>0.99999998999999995</v>
+        <v>1000</v>
       </c>
       <c r="E83">
-        <v>0.08</v>
+        <v>1E-3</v>
       </c>
       <c r="F83" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>251</v>
+        <v>140</v>
       </c>
       <c r="B84" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C84">
+        <v>-6.3</v>
+      </c>
+      <c r="D84">
+        <v>6.3</v>
+      </c>
+      <c r="E84">
         <v>0</v>
       </c>
-      <c r="D84">
-        <v>0.99999998999999995</v>
-      </c>
-      <c r="E84">
-        <v>2E-3</v>
-      </c>
       <c r="F84" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
+        <v>141</v>
+      </c>
+      <c r="B85" t="s">
+        <v>218</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>239</v>
+      </c>
+      <c r="B86" t="s">
+        <v>220</v>
+      </c>
+      <c r="C86">
+        <v>-1.5</v>
+      </c>
+      <c r="D86">
+        <v>1.5</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>246</v>
+      </c>
+      <c r="B87" t="s">
+        <v>221</v>
+      </c>
+      <c r="C87">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D87">
+        <v>99999999</v>
+      </c>
+      <c r="E87">
+        <v>200</v>
+      </c>
+      <c r="F87" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>247</v>
+      </c>
+      <c r="B88" t="s">
+        <v>223</v>
+      </c>
+      <c r="C88">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D88">
+        <v>0.99999998999999995</v>
+      </c>
+      <c r="E88">
+        <v>1.6659999999999999E-3</v>
+      </c>
+      <c r="F88" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>248</v>
+      </c>
+      <c r="B89" t="s">
+        <v>225</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0.99999998999999995</v>
+      </c>
+      <c r="E89">
+        <v>1.25E-3</v>
+      </c>
+      <c r="F89" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>249</v>
+      </c>
+      <c r="B90" t="s">
+        <v>227</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>9999.9999000000007</v>
+      </c>
+      <c r="E90">
+        <v>0.45</v>
+      </c>
+      <c r="F90" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>250</v>
+      </c>
+      <c r="B91" t="s">
+        <v>229</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0.99999998999999995</v>
+      </c>
+      <c r="E91">
+        <v>0.08</v>
+      </c>
+      <c r="F91" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>251</v>
+      </c>
+      <c r="B92" t="s">
+        <v>231</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0.99999998999999995</v>
+      </c>
+      <c r="E92">
+        <v>2E-3</v>
+      </c>
+      <c r="F92" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93">
         <v>252</v>
       </c>
-      <c r="B85" t="s">
-        <v>216</v>
-      </c>
-      <c r="C85">
+      <c r="B93" t="s">
+        <v>233</v>
+      </c>
+      <c r="C93">
         <v>-2</v>
       </c>
-      <c r="D85">
+      <c r="D93">
         <v>2</v>
       </c>
-      <c r="E85">
+      <c r="E93">
         <v>0.65</v>
       </c>
-      <c r="F85" t="s">
-        <v>217</v>
+      <c r="F93" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>